<commit_message>
new fellows, be nice alright?
</commit_message>
<xml_diff>
--- a/SNP位點挑選資訊_自製表格_Mika_AS.xlsx
+++ b/SNP位點挑選資訊_自製表格_Mika_AS.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikali\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mikali\Desktop\20240723\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36502ED5-FD39-4591-98B7-7D4760D1EED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BFEB67A-D434-4166-9B13-9429BAA5E161}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{E97A958B-F40C-4998-BD87-385C687588E0}"/>
   </bookViews>
@@ -25,12 +25,231 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>Gene ID</t>
+  </si>
+  <si>
+    <t>Chromosome</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>genome version (GRCh37 or GRCh38)</t>
+  </si>
+  <si>
+    <t>ref allele</t>
+  </si>
+  <si>
+    <t>minor allele (Alternative)</t>
+  </si>
+  <si>
+    <t>MAF</t>
+  </si>
+  <si>
+    <t>Odds Ratio (OR, GWAS)</t>
+  </si>
+  <si>
+    <t>Population</t>
+  </si>
+  <si>
+    <t>其他資訊自行增列</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Microsoft YaHei"/>
+        <family val="2"/>
+      </rPr>
+      <t>變異位點</t>
+    </r>
+  </si>
+  <si>
+    <t>A.A 
+change</t>
+  </si>
+  <si>
+    <t>Inheritance mode</t>
+  </si>
+  <si>
+    <r>
+      <t>Original Source 
+(GWAS</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>、</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>dbSNP</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>、Ensembl、papers</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>是否存在同點位</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>&amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>具致病性的紀錄</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> 
+(</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>此處多附加相隔</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1bp </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="微軟正黑體"/>
+        <family val="2"/>
+        <charset val="136"/>
+      </rPr>
+      <t>的致病位點紀錄</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>MAF TWB_TW
+(n=~1500)</t>
+  </si>
+  <si>
+    <t>MAF 1000G_EAS
+(n=504)</t>
+  </si>
+  <si>
+    <t>綜合判斷</t>
+  </si>
+  <si>
+    <t> PRS</t>
+  </si>
+  <si>
+    <t>EFO</t>
+  </si>
+  <si>
+    <t>說明2</t>
+  </si>
+  <si>
+    <t>pValue</t>
+  </si>
+  <si>
+    <t>dbSNP ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Gene Label</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="180" formatCode="0.000%"/>
+  </numFmts>
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -46,16 +265,59 @@
       <charset val="136"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="新細明體"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Microsoft YaHei"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="微軟正黑體"/>
+      <family val="2"/>
+      <charset val="136"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -63,19 +325,69 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
+    <cellStyle name="一般 2" xfId="2" xr:uid="{8C8C6BDC-2D58-4418-A0BD-89873430CB24}"/>
+    <cellStyle name="一般 3" xfId="1" xr:uid="{104783E6-E13F-4C05-B430-1C85F000E792}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -387,14 +699,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B141AFE-70C6-4881-AC9F-CC763A5EE5B5}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:25" ht="89.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="M1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="R1" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="S1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="T1" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="U1" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="V1" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="W1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="X1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>